<commit_message>
Actualizacion nov y correccion de archivos y permisos
</commit_message>
<xml_diff>
--- a/xlsx/a69_f11UPPachuca.xlsx
+++ b/xlsx/a69_f11UPPachuca.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Desktop\3er Trimestre Fracciones faltantes\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8655"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8355"/>
   </bookViews>
   <sheets>
     <sheet name="Reporte de Formatos" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="171">
   <si>
     <t>44234</t>
   </si>
@@ -220,9 +220,6 @@
     <t>Profesor por asignatura A</t>
   </si>
   <si>
-    <t>http://www.upp.edu.mx/normatividad/wp-content/uploads/2014/11/Reglamento-Interno-Mar_2014.pdf</t>
-  </si>
-  <si>
     <t>Albino</t>
   </si>
   <si>
@@ -511,6 +508,9 @@
     <t>Argueta</t>
   </si>
   <si>
+    <t>La institución no genera números de contratos para el personal contratados por honorarios, ni se generan prestaciones de ningún tipo. No se ha concluido el proceso, debido a que el contrato aún se encuentra en proceso de firma,ya que derivado de la contingencia sanitaria que se tiene actualmente, el proceso de firma es más tardado.</t>
+  </si>
+  <si>
     <t>La institución no genera números de contratos para el personal contratados por honorarios, ni se generan prestaciones de ningún tipo.</t>
   </si>
   <si>
@@ -523,118 +523,19 @@
     <t>Barrera</t>
   </si>
   <si>
+    <t>La institución no genera números de contratos para el personal contratados por honorarios. No se ha concluido el proceso, debido a que el contrato aún se encuentra en proceso de firma,ya que derivado de la contingencia sanitaria que se tiene actualmente, el proceso de firma es más tardado.</t>
+  </si>
+  <si>
     <t>ISSSTE</t>
   </si>
   <si>
-    <t>La institución no genera números de contratos para el personal contratados por honorarios, ni se generan prestaciones de ningún tipo. En el caso de la profesora, no se ha firmado el contrato aún, y derivado de la contingencia sanitaria que se tiene actualmente, por lo cual no se ha concluido el trámite de firma.</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/13JzDAOtd-C4b76iD7fwNYi38K9vrjHs6/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1Ip1ZbdjNoiynWAnbgYxPVEhxUGL4Q5GC/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/183xOEA8EqZMr87g_R9D_GPAPDCDBXnNn/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1cxvxLxvmiTyjK6tjC3GifF4cjm3P3E53/view?usp=sharing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La institución no genera números de contratos para el personal contratados por honorarios, ni se generan prestaciones de ningún tipo. </t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1TJqjEdxnodxjJXxOq5SffbK7MU53oNKM/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/12K0wkJEpM88j2UtX-HeiJ1kXD_PPneoW/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1pgdxJErrYEimwuSQln8ffIeWfWqssbSm/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1cNQ4aVTruh4VckfRfIXsAmmyaYe14TiN/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1GMIe18QNrK35SsYduoNTYkAWvRm7ULUZ/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1ADbq-qI4BCX-r4pZsliO8wSoBu2bEpqL/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1B4JtJz945jshB5koItcXYxBOEe1b_ieX/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1CwjBnmcPc06PgPQhrDcgKUt3-fpUs4pQ/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/10NYYDDNYx2CvlC5fygBKRiWaKOeFonzM/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1VDS-F-F29NxX-FCd9ct0d1CyuvLBPSkM/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1OQRJKirPC8ETg7Vid2HXbugWHarP_fyK/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1kGog23lllp9fc833sNA_Oy9t3aTU1CbY/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1rBnHOoJjzltkIk8dG_UhHAyDT_dOFB1H/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1qvHZIhb1-M6QaAuYdDmbpkVu9La25ZDC/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/11b1gv7f9Dxy45pF-DR2J9Ymd3Z-et96l/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/12YujP8qooPjFiorbZXbfkI79aBm2ySyJ/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1_kKtGgYWqkpap_cbdXmAHhQOGLmn4GaA/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1lZbOgxQvmvwawsSlGVDu3ox4h0H-N8v1/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1G3qQv1b_mVON6DdW4da8FlQ7r6Ta9jpQ/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1Ivzzj4HZDCwhr7SgX3cigDKrBfbIF27a/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1Th-zPl4nnWKol71Pje6ajJahWPfGBC9m/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1qIlYSB6FFJ71A1lP7M4KrGGK67VnORDv/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1vQlMj5OcdzJxjUNZLScX6YaWtzgZCY0T/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1W3F3RhJySBr0cjJagu_y8bAztngrdOhJ/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1shoigk7geM1bvX9cB7zYFzKiIeJKpDhF/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1wU1TZMY8UvbyLRPvWyizIy0bWQ9Calin/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/119eDeB8RcXd3s1p0nIR5FGCfGwEu-9IO/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1g0Vw6rjLJ6oeFMQ3wFbUc6V9Snkfi5bx/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1OyzNVRFsqEAQCZ0wYbUlGRjEEPnjszxl/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1YULBExIKUPBvp5UPgmOexYtBrIwQ5pjy/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1PxWETBA6cre32Hf_oJ506Iz-LmM529ir/view?usp=sharing</t>
+    <t>https://drive.google.com/file/d/1ghGfQVCnPtBy4ZwW2oaScnx67pCDuad0/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1O1oAlRbipeklRItiZUbAOxxy8__Xo1dH/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>http://www.upp.edu.mx/normatividad/files/interna/reglamentos/reglamento-interno-mar_2014.pdf</t>
   </si>
 </sst>
 </file>
@@ -727,7 +628,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -775,6 +676,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -784,12 +688,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1073,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="O2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q44" sqref="Q44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,18 +980,18 @@
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="86.140625" customWidth="1"/>
+    <col min="10" max="10" width="29.5703125" customWidth="1"/>
     <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="41.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" style="18" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="71.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="73.140625" bestFit="1" customWidth="1"/>
@@ -1109,39 +1007,39 @@
       <c r="O1"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="19" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="19" t="s">
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
       <c r="O2"/>
     </row>
-    <row r="3" spans="1:21" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
       <c r="O3"/>
     </row>
     <row r="4" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
@@ -1209,7 +1107,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1275,29 +1173,29 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="20"/>
-      <c r="S6" s="20"/>
-      <c r="T6" s="20"/>
-      <c r="U6" s="20"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21"/>
+      <c r="S6" s="21"/>
+      <c r="T6" s="21"/>
+      <c r="U6" s="21"/>
     </row>
     <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1364,7 +1262,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2020</v>
       </c>
@@ -1390,9 +1288,7 @@
         <v>63</v>
       </c>
       <c r="I8" s="13"/>
-      <c r="J8" s="18" t="s">
-        <v>168</v>
-      </c>
+      <c r="J8" s="14"/>
       <c r="K8" s="7">
         <v>44081</v>
       </c>
@@ -1409,10 +1305,10 @@
         <v>18144</v>
       </c>
       <c r="P8" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R8" s="4" t="s">
         <v>60</v>
@@ -1424,10 +1320,10 @@
         <v>44114</v>
       </c>
       <c r="U8" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2020</v>
       </c>
@@ -1444,16 +1340,16 @@
         <v>121001</v>
       </c>
       <c r="F9" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="H9" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="13" t="s">
-        <v>68</v>
-      </c>
       <c r="I9" s="13"/>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="19" t="s">
         <v>169</v>
       </c>
       <c r="K9" s="7">
@@ -1463,7 +1359,7 @@
         <v>44196</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N9" s="15">
         <v>22738.5</v>
@@ -1473,7 +1369,7 @@
       </c>
       <c r="P9" s="8"/>
       <c r="Q9" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R9" s="4" t="s">
         <v>60</v>
@@ -1488,7 +1384,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>2020</v>
       </c>
@@ -1505,17 +1401,17 @@
         <v>121001</v>
       </c>
       <c r="F10" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="H10" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="H10" s="13" t="s">
-        <v>72</v>
-      </c>
       <c r="I10" s="13"/>
-      <c r="J10" s="18" t="s">
-        <v>170</v>
+      <c r="J10" s="19" t="s">
+        <v>168</v>
       </c>
       <c r="K10" s="7">
         <v>44013</v>
@@ -1524,7 +1420,7 @@
         <v>44196</v>
       </c>
       <c r="M10" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N10" s="15">
         <v>14053.34</v>
@@ -1534,7 +1430,7 @@
       </c>
       <c r="P10" s="8"/>
       <c r="Q10" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R10" s="4" t="s">
         <v>60</v>
@@ -1549,7 +1445,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>2020</v>
       </c>
@@ -1566,18 +1462,16 @@
         <v>121001</v>
       </c>
       <c r="F11" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="H11" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="H11" s="13" t="s">
-        <v>76</v>
-      </c>
       <c r="I11" s="13"/>
-      <c r="J11" s="18" t="s">
-        <v>171</v>
-      </c>
+      <c r="J11" s="14"/>
       <c r="K11" s="7">
         <v>44081</v>
       </c>
@@ -1585,7 +1479,7 @@
         <v>44183</v>
       </c>
       <c r="M11" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N11" s="15">
         <v>9881.16</v>
@@ -1594,10 +1488,10 @@
         <v>27783</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q11" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R11" s="4" t="s">
         <v>60</v>
@@ -1609,7 +1503,7 @@
         <v>44114</v>
       </c>
       <c r="U11" s="12" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="75" x14ac:dyDescent="0.25">
@@ -1629,13 +1523,13 @@
         <v>121001</v>
       </c>
       <c r="F12" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="H12" s="13" t="s">
         <v>79</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>80</v>
       </c>
       <c r="I12" s="13"/>
       <c r="J12" s="14"/>
@@ -1655,10 +1549,10 @@
         <v>19278</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q12" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R12" s="4" t="s">
         <v>60</v>
@@ -1670,10 +1564,10 @@
         <v>44114</v>
       </c>
       <c r="U12" s="12" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>2020</v>
       </c>
@@ -1690,18 +1584,16 @@
         <v>121001</v>
       </c>
       <c r="F13" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="H13" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="H13" s="13" t="s">
-        <v>83</v>
-      </c>
       <c r="I13" s="13"/>
-      <c r="J13" s="18" t="s">
-        <v>173</v>
-      </c>
+      <c r="J13" s="14"/>
       <c r="K13" s="7">
         <v>44081</v>
       </c>
@@ -1718,10 +1610,10 @@
         <v>22680</v>
       </c>
       <c r="P13" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q13" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R13" s="4" t="s">
         <v>60</v>
@@ -1733,10 +1625,10 @@
         <v>44114</v>
       </c>
       <c r="U13" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>2020</v>
       </c>
@@ -1753,18 +1645,16 @@
         <v>121001</v>
       </c>
       <c r="F14" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G14" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="H14" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="H14" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="I14" s="13"/>
-      <c r="J14" s="18" t="s">
-        <v>174</v>
-      </c>
+      <c r="J14" s="14"/>
       <c r="K14" s="7">
         <v>44081</v>
       </c>
@@ -1781,10 +1671,10 @@
         <v>22680</v>
       </c>
       <c r="P14" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q14" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R14" s="4" t="s">
         <v>60</v>
@@ -1796,10 +1686,10 @@
         <v>44114</v>
       </c>
       <c r="U14" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>2020</v>
       </c>
@@ -1825,9 +1715,7 @@
         <v>165</v>
       </c>
       <c r="I15" s="13"/>
-      <c r="J15" s="18" t="s">
-        <v>175</v>
-      </c>
+      <c r="J15" s="14"/>
       <c r="K15" s="7">
         <v>44081</v>
       </c>
@@ -1845,7 +1733,7 @@
       </c>
       <c r="P15" s="8"/>
       <c r="Q15" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R15" s="4" t="s">
         <v>60</v>
@@ -1857,10 +1745,10 @@
         <v>44114</v>
       </c>
       <c r="U15" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>2020</v>
       </c>
@@ -1877,18 +1765,16 @@
         <v>121001</v>
       </c>
       <c r="F16" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="H16" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="H16" s="13" t="s">
-        <v>89</v>
-      </c>
       <c r="I16" s="13"/>
-      <c r="J16" s="18" t="s">
-        <v>176</v>
-      </c>
+      <c r="J16" s="14"/>
       <c r="K16" s="7">
         <v>44081</v>
       </c>
@@ -1905,10 +1791,10 @@
         <v>22680</v>
       </c>
       <c r="P16" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q16" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R16" s="4" t="s">
         <v>60</v>
@@ -1920,10 +1806,10 @@
         <v>44114</v>
       </c>
       <c r="U16" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>2020</v>
       </c>
@@ -1940,18 +1826,16 @@
         <v>121001</v>
       </c>
       <c r="F17" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="H17" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="H17" s="13" t="s">
-        <v>92</v>
-      </c>
       <c r="I17" s="13"/>
-      <c r="J17" s="18" t="s">
-        <v>177</v>
-      </c>
+      <c r="J17" s="14"/>
       <c r="K17" s="7">
         <v>44081</v>
       </c>
@@ -1968,10 +1852,10 @@
         <v>22680</v>
       </c>
       <c r="P17" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q17" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R17" s="4" t="s">
         <v>60</v>
@@ -1983,10 +1867,10 @@
         <v>44114</v>
       </c>
       <c r="U17" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>2020</v>
       </c>
@@ -2003,18 +1887,16 @@
         <v>121001</v>
       </c>
       <c r="F18" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="G18" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="H18" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="H18" s="13" t="s">
-        <v>95</v>
-      </c>
       <c r="I18" s="13"/>
-      <c r="J18" s="18" t="s">
-        <v>178</v>
-      </c>
+      <c r="J18" s="14"/>
       <c r="K18" s="7">
         <v>44081</v>
       </c>
@@ -2022,7 +1904,7 @@
         <v>44183</v>
       </c>
       <c r="M18" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N18" s="15">
         <v>9881.16</v>
@@ -2031,10 +1913,10 @@
         <v>27783</v>
       </c>
       <c r="P18" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R18" s="4" t="s">
         <v>60</v>
@@ -2046,10 +1928,10 @@
         <v>44114</v>
       </c>
       <c r="U18" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>2020</v>
       </c>
@@ -2066,18 +1948,16 @@
         <v>121001</v>
       </c>
       <c r="F19" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="G19" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="H19" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="H19" s="13" t="s">
-        <v>98</v>
-      </c>
       <c r="I19" s="13"/>
-      <c r="J19" s="18" t="s">
-        <v>179</v>
-      </c>
+      <c r="J19" s="14"/>
       <c r="K19" s="7">
         <v>44081</v>
       </c>
@@ -2094,10 +1974,10 @@
         <v>22680</v>
       </c>
       <c r="P19" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q19" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R19" s="4" t="s">
         <v>60</v>
@@ -2109,10 +1989,10 @@
         <v>44114</v>
       </c>
       <c r="U19" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>2020</v>
       </c>
@@ -2129,18 +2009,16 @@
         <v>121001</v>
       </c>
       <c r="F20" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="H20" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="H20" s="13" t="s">
-        <v>101</v>
-      </c>
       <c r="I20" s="13"/>
-      <c r="J20" s="18" t="s">
-        <v>180</v>
-      </c>
+      <c r="J20" s="14"/>
       <c r="K20" s="7">
         <v>44081</v>
       </c>
@@ -2157,10 +2035,10 @@
         <v>15876</v>
       </c>
       <c r="P20" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q20" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R20" s="4" t="s">
         <v>60</v>
@@ -2172,10 +2050,10 @@
         <v>44114</v>
       </c>
       <c r="U20" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>2020</v>
       </c>
@@ -2192,18 +2070,16 @@
         <v>121001</v>
       </c>
       <c r="F21" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="G21" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="H21" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="H21" s="13" t="s">
-        <v>104</v>
-      </c>
       <c r="I21" s="13"/>
-      <c r="J21" s="18" t="s">
-        <v>181</v>
-      </c>
+      <c r="J21" s="14"/>
       <c r="K21" s="7">
         <v>44081</v>
       </c>
@@ -2211,7 +2087,7 @@
         <v>44183</v>
       </c>
       <c r="M21" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N21" s="15">
         <v>7391.7</v>
@@ -2220,10 +2096,10 @@
         <v>21168</v>
       </c>
       <c r="P21" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q21" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R21" s="4" t="s">
         <v>60</v>
@@ -2235,10 +2111,10 @@
         <v>44114</v>
       </c>
       <c r="U21" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>2020</v>
       </c>
@@ -2255,18 +2131,16 @@
         <v>121001</v>
       </c>
       <c r="F22" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="G22" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="H22" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="H22" s="13" t="s">
-        <v>107</v>
-      </c>
       <c r="I22" s="13"/>
-      <c r="J22" s="18" t="s">
-        <v>182</v>
-      </c>
+      <c r="J22" s="14"/>
       <c r="K22" s="7">
         <v>44081</v>
       </c>
@@ -2283,10 +2157,10 @@
         <v>22680</v>
       </c>
       <c r="P22" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q22" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R22" s="4" t="s">
         <v>60</v>
@@ -2298,10 +2172,10 @@
         <v>44114</v>
       </c>
       <c r="U22" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>2020</v>
       </c>
@@ -2318,18 +2192,16 @@
         <v>121001</v>
       </c>
       <c r="F23" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="G23" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="H23" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="H23" s="13" t="s">
-        <v>110</v>
-      </c>
       <c r="I23" s="13"/>
-      <c r="J23" s="18" t="s">
-        <v>183</v>
-      </c>
+      <c r="J23" s="14"/>
       <c r="K23" s="7">
         <v>44081</v>
       </c>
@@ -2346,10 +2218,10 @@
         <v>22680</v>
       </c>
       <c r="P23" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q23" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R23" s="4" t="s">
         <v>60</v>
@@ -2361,10 +2233,10 @@
         <v>44114</v>
       </c>
       <c r="U23" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>2020</v>
       </c>
@@ -2381,18 +2253,16 @@
         <v>121001</v>
       </c>
       <c r="F24" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G24" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="H24" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="H24" s="13" t="s">
-        <v>113</v>
-      </c>
       <c r="I24" s="13"/>
-      <c r="J24" s="18" t="s">
-        <v>184</v>
-      </c>
+      <c r="J24" s="14"/>
       <c r="K24" s="7">
         <v>44081</v>
       </c>
@@ -2409,10 +2279,10 @@
         <v>17010</v>
       </c>
       <c r="P24" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q24" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R24" s="4" t="s">
         <v>60</v>
@@ -2424,10 +2294,10 @@
         <v>44114</v>
       </c>
       <c r="U24" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>2020</v>
       </c>
@@ -2444,18 +2314,16 @@
         <v>121001</v>
       </c>
       <c r="F25" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G25" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="G25" s="13" t="s">
+      <c r="H25" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="H25" s="13" t="s">
-        <v>116</v>
-      </c>
       <c r="I25" s="13"/>
-      <c r="J25" s="18" t="s">
-        <v>185</v>
-      </c>
+      <c r="J25" s="14"/>
       <c r="K25" s="7">
         <v>44081</v>
       </c>
@@ -2472,10 +2340,10 @@
         <v>22680</v>
       </c>
       <c r="P25" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q25" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R25" s="4" t="s">
         <v>60</v>
@@ -2487,10 +2355,10 @@
         <v>44114</v>
       </c>
       <c r="U25" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>2020</v>
       </c>
@@ -2507,18 +2375,16 @@
         <v>121001</v>
       </c>
       <c r="F26" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="G26" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="G26" s="13" t="s">
+      <c r="H26" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="H26" s="13" t="s">
-        <v>119</v>
-      </c>
       <c r="I26" s="13"/>
-      <c r="J26" s="18" t="s">
-        <v>186</v>
-      </c>
+      <c r="J26" s="14"/>
       <c r="K26" s="7">
         <v>44081</v>
       </c>
@@ -2535,10 +2401,10 @@
         <v>22680</v>
       </c>
       <c r="P26" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q26" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R26" s="4" t="s">
         <v>60</v>
@@ -2550,10 +2416,10 @@
         <v>44114</v>
       </c>
       <c r="U26" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>2020</v>
       </c>
@@ -2570,18 +2436,16 @@
         <v>121001</v>
       </c>
       <c r="F27" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="G27" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="H27" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="H27" s="13" t="s">
-        <v>122</v>
-      </c>
       <c r="I27" s="13"/>
-      <c r="J27" s="18" t="s">
-        <v>187</v>
-      </c>
+      <c r="J27" s="14"/>
       <c r="K27" s="7">
         <v>44081</v>
       </c>
@@ -2589,7 +2453,7 @@
         <v>44183</v>
       </c>
       <c r="M27" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N27" s="15">
         <v>8354.82</v>
@@ -2598,10 +2462,10 @@
         <v>23814</v>
       </c>
       <c r="P27" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q27" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R27" s="4" t="s">
         <v>60</v>
@@ -2613,10 +2477,10 @@
         <v>44114</v>
       </c>
       <c r="U27" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>2020</v>
       </c>
@@ -2633,18 +2497,16 @@
         <v>121001</v>
       </c>
       <c r="F28" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G28" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="H28" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="H28" s="13" t="s">
-        <v>125</v>
-      </c>
       <c r="I28" s="13"/>
-      <c r="J28" s="18" t="s">
-        <v>188</v>
-      </c>
+      <c r="J28" s="14"/>
       <c r="K28" s="7">
         <v>44081</v>
       </c>
@@ -2661,10 +2523,10 @@
         <v>22680</v>
       </c>
       <c r="P28" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q28" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R28" s="4" t="s">
         <v>60</v>
@@ -2676,10 +2538,10 @@
         <v>44114</v>
       </c>
       <c r="U28" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>2020</v>
       </c>
@@ -2696,18 +2558,16 @@
         <v>121001</v>
       </c>
       <c r="F29" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G29" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="G29" s="13" t="s">
+      <c r="H29" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="H29" s="13" t="s">
-        <v>128</v>
-      </c>
       <c r="I29" s="13"/>
-      <c r="J29" s="18" t="s">
-        <v>189</v>
-      </c>
+      <c r="J29" s="14"/>
       <c r="K29" s="7">
         <v>44081</v>
       </c>
@@ -2724,10 +2584,10 @@
         <v>17010</v>
       </c>
       <c r="P29" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q29" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R29" s="4" t="s">
         <v>60</v>
@@ -2739,10 +2599,10 @@
         <v>44114</v>
       </c>
       <c r="U29" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>2020</v>
       </c>
@@ -2759,18 +2619,16 @@
         <v>121001</v>
       </c>
       <c r="F30" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H30" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="G30" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>130</v>
-      </c>
       <c r="I30" s="13"/>
-      <c r="J30" s="18" t="s">
-        <v>190</v>
-      </c>
+      <c r="J30" s="14"/>
       <c r="K30" s="7">
         <v>44081</v>
       </c>
@@ -2778,7 +2636,7 @@
         <v>44183</v>
       </c>
       <c r="M30" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N30" s="15">
         <v>7873.24</v>
@@ -2787,10 +2645,10 @@
         <v>22491</v>
       </c>
       <c r="P30" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q30" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R30" s="4" t="s">
         <v>60</v>
@@ -2802,10 +2660,10 @@
         <v>44114</v>
       </c>
       <c r="U30" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>2020</v>
       </c>
@@ -2822,18 +2680,16 @@
         <v>121001</v>
       </c>
       <c r="F31" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="G31" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="G31" s="13" t="s">
+      <c r="H31" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H31" s="13" t="s">
-        <v>133</v>
-      </c>
       <c r="I31" s="13"/>
-      <c r="J31" s="18" t="s">
-        <v>191</v>
-      </c>
+      <c r="J31" s="14"/>
       <c r="K31" s="7">
         <v>44081</v>
       </c>
@@ -2850,10 +2706,10 @@
         <v>22680</v>
       </c>
       <c r="P31" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q31" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R31" s="4" t="s">
         <v>60</v>
@@ -2865,10 +2721,10 @@
         <v>44114</v>
       </c>
       <c r="U31" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>2020</v>
       </c>
@@ -2885,18 +2741,16 @@
         <v>121001</v>
       </c>
       <c r="F32" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="G32" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="G32" s="13" t="s">
-        <v>135</v>
-      </c>
       <c r="H32" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I32" s="13"/>
-      <c r="J32" s="18" t="s">
-        <v>192</v>
-      </c>
+      <c r="J32" s="14"/>
       <c r="K32" s="7">
         <v>44081</v>
       </c>
@@ -2913,10 +2767,10 @@
         <v>22680</v>
       </c>
       <c r="P32" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q32" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R32" s="4" t="s">
         <v>60</v>
@@ -2928,10 +2782,10 @@
         <v>44114</v>
       </c>
       <c r="U32" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>2020</v>
       </c>
@@ -2948,18 +2802,16 @@
         <v>121001</v>
       </c>
       <c r="F33" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="G33" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="G33" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="H33" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I33" s="13"/>
-      <c r="J33" s="18" t="s">
-        <v>193</v>
-      </c>
+      <c r="J33" s="14"/>
       <c r="K33" s="7">
         <v>44081</v>
       </c>
@@ -2976,10 +2828,10 @@
         <v>22680</v>
       </c>
       <c r="P33" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q33" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R33" s="4" t="s">
         <v>60</v>
@@ -2991,10 +2843,10 @@
         <v>44114</v>
       </c>
       <c r="U33" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>2020</v>
       </c>
@@ -3011,18 +2863,16 @@
         <v>121001</v>
       </c>
       <c r="F34" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="G34" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="G34" s="13" t="s">
+      <c r="H34" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="H34" s="13" t="s">
-        <v>140</v>
-      </c>
       <c r="I34" s="13"/>
-      <c r="J34" s="18" t="s">
-        <v>194</v>
-      </c>
+      <c r="J34" s="14"/>
       <c r="K34" s="7">
         <v>44081</v>
       </c>
@@ -3039,10 +2889,10 @@
         <v>23814</v>
       </c>
       <c r="P34" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q34" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R34" s="4" t="s">
         <v>60</v>
@@ -3054,10 +2904,10 @@
         <v>44114</v>
       </c>
       <c r="U34" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>2020</v>
       </c>
@@ -3074,18 +2924,16 @@
         <v>121001</v>
       </c>
       <c r="F35" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="H35" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="G35" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="H35" s="13" t="s">
-        <v>142</v>
-      </c>
       <c r="I35" s="13"/>
-      <c r="J35" s="18" t="s">
-        <v>195</v>
-      </c>
+      <c r="J35" s="14"/>
       <c r="K35" s="7">
         <v>44081</v>
       </c>
@@ -3093,7 +2941,7 @@
         <v>44183</v>
       </c>
       <c r="M35" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N35" s="15">
         <v>8354.82</v>
@@ -3102,10 +2950,10 @@
         <v>23814</v>
       </c>
       <c r="P35" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q35" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R35" s="4" t="s">
         <v>60</v>
@@ -3117,10 +2965,10 @@
         <v>44114</v>
       </c>
       <c r="U35" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>2020</v>
       </c>
@@ -3137,18 +2985,16 @@
         <v>121001</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G36" s="13" t="s">
         <v>63</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I36" s="13"/>
-      <c r="J36" s="18" t="s">
-        <v>196</v>
-      </c>
+      <c r="J36" s="14"/>
       <c r="K36" s="7">
         <v>44081</v>
       </c>
@@ -3156,7 +3002,7 @@
         <v>44183</v>
       </c>
       <c r="M36" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N36" s="15">
         <v>9881.16</v>
@@ -3165,10 +3011,10 @@
         <v>27783</v>
       </c>
       <c r="P36" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q36" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R36" s="4" t="s">
         <v>60</v>
@@ -3180,10 +3026,10 @@
         <v>44114</v>
       </c>
       <c r="U36" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>2020</v>
       </c>
@@ -3200,18 +3046,16 @@
         <v>121001</v>
       </c>
       <c r="F37" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="G37" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="G37" s="13" t="s">
-        <v>146</v>
-      </c>
       <c r="H37" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I37" s="13"/>
-      <c r="J37" s="18" t="s">
-        <v>197</v>
-      </c>
+      <c r="J37" s="14"/>
       <c r="K37" s="7">
         <v>44081</v>
       </c>
@@ -3228,10 +3072,10 @@
         <v>17010</v>
       </c>
       <c r="P37" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q37" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R37" s="4" t="s">
         <v>60</v>
@@ -3243,10 +3087,10 @@
         <v>44114</v>
       </c>
       <c r="U37" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>2020</v>
       </c>
@@ -3263,18 +3107,16 @@
         <v>121001</v>
       </c>
       <c r="F38" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="H38" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="G38" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="H38" s="13" t="s">
-        <v>148</v>
-      </c>
       <c r="I38" s="13"/>
-      <c r="J38" s="18" t="s">
-        <v>198</v>
-      </c>
+      <c r="J38" s="14"/>
       <c r="K38" s="7">
         <v>44081</v>
       </c>
@@ -3291,10 +3133,10 @@
         <v>22680</v>
       </c>
       <c r="P38" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q38" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R38" s="4" t="s">
         <v>60</v>
@@ -3306,10 +3148,10 @@
         <v>44114</v>
       </c>
       <c r="U38" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>2020</v>
       </c>
@@ -3326,18 +3168,16 @@
         <v>121001</v>
       </c>
       <c r="F39" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="G39" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="G39" s="13" t="s">
+      <c r="H39" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="H39" s="13" t="s">
-        <v>151</v>
-      </c>
       <c r="I39" s="13"/>
-      <c r="J39" s="18" t="s">
-        <v>199</v>
-      </c>
+      <c r="J39" s="14"/>
       <c r="K39" s="7">
         <v>44081</v>
       </c>
@@ -3354,10 +3194,10 @@
         <v>22680</v>
       </c>
       <c r="P39" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q39" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R39" s="4" t="s">
         <v>60</v>
@@ -3369,10 +3209,10 @@
         <v>44114</v>
       </c>
       <c r="U39" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>2020</v>
       </c>
@@ -3389,18 +3229,16 @@
         <v>121001</v>
       </c>
       <c r="F40" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="G40" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G40" s="13" t="s">
-        <v>153</v>
-      </c>
       <c r="H40" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I40" s="13"/>
-      <c r="J40" s="18" t="s">
-        <v>200</v>
-      </c>
+      <c r="J40" s="14"/>
       <c r="K40" s="7">
         <v>44081</v>
       </c>
@@ -3417,10 +3255,10 @@
         <v>22680</v>
       </c>
       <c r="P40" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q40" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R40" s="4" t="s">
         <v>60</v>
@@ -3432,10 +3270,10 @@
         <v>44114</v>
       </c>
       <c r="U40" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>2020</v>
       </c>
@@ -3452,18 +3290,16 @@
         <v>121001</v>
       </c>
       <c r="F41" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="G41" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="G41" s="13" t="s">
+      <c r="H41" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="H41" s="13" t="s">
-        <v>156</v>
-      </c>
       <c r="I41" s="13"/>
-      <c r="J41" s="18" t="s">
-        <v>201</v>
-      </c>
+      <c r="J41" s="14"/>
       <c r="K41" s="7">
         <v>44081</v>
       </c>
@@ -3471,7 +3307,7 @@
         <v>44183</v>
       </c>
       <c r="M41" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N41" s="15">
         <v>9365.9599999999991</v>
@@ -3480,10 +3316,10 @@
         <v>26460</v>
       </c>
       <c r="P41" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q41" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R41" s="4" t="s">
         <v>60</v>
@@ -3495,10 +3331,10 @@
         <v>44114</v>
       </c>
       <c r="U41" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>2020</v>
       </c>
@@ -3515,18 +3351,16 @@
         <v>121001</v>
       </c>
       <c r="F42" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I42" s="13"/>
-      <c r="J42" s="18" t="s">
-        <v>202</v>
-      </c>
+      <c r="J42" s="14"/>
       <c r="K42" s="7">
         <v>44081</v>
       </c>
@@ -3534,7 +3368,7 @@
         <v>44183</v>
       </c>
       <c r="M42" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N42" s="15">
         <v>10859.58</v>
@@ -3543,10 +3377,10 @@
         <v>30240</v>
       </c>
       <c r="P42" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q42" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R42" s="4" t="s">
         <v>60</v>
@@ -3558,10 +3392,10 @@
         <v>44114</v>
       </c>
       <c r="U42" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>2020</v>
       </c>
@@ -3578,18 +3412,16 @@
         <v>121001</v>
       </c>
       <c r="F43" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="G43" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="G43" s="13" t="s">
+      <c r="H43" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="H43" s="13" t="s">
-        <v>161</v>
-      </c>
       <c r="I43" s="16"/>
-      <c r="J43" s="18" t="s">
-        <v>203</v>
-      </c>
+      <c r="J43" s="17"/>
       <c r="K43" s="7">
         <v>44081</v>
       </c>
@@ -3606,10 +3438,10 @@
         <v>22080</v>
       </c>
       <c r="P43" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="Q43" s="9" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="R43" s="4" t="s">
         <v>60</v>
@@ -3621,7 +3453,7 @@
         <v>44114</v>
       </c>
       <c r="U43" s="12" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -3635,85 +3467,52 @@
     <mergeCell ref="G3:I3"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D8:D43">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D8:D200">
       <formula1>Hidden_13</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="Q8:Q31" r:id="rId1" display="http://www.upp.edu.mx/normatividad/wp-content/uploads/2014/11/Reglamento-Interno-Mar_2014.pdf"/>
-    <hyperlink ref="Q9" r:id="rId2"/>
-    <hyperlink ref="Q10" r:id="rId3"/>
-    <hyperlink ref="Q11" r:id="rId4"/>
-    <hyperlink ref="Q13" r:id="rId5"/>
-    <hyperlink ref="Q14" r:id="rId6"/>
-    <hyperlink ref="Q16" r:id="rId7"/>
-    <hyperlink ref="Q17" r:id="rId8"/>
-    <hyperlink ref="Q18" r:id="rId9"/>
-    <hyperlink ref="Q19" r:id="rId10"/>
-    <hyperlink ref="Q20" r:id="rId11"/>
-    <hyperlink ref="Q21" r:id="rId12"/>
-    <hyperlink ref="Q22" r:id="rId13"/>
-    <hyperlink ref="Q23" r:id="rId14"/>
-    <hyperlink ref="Q24" r:id="rId15"/>
-    <hyperlink ref="Q25" r:id="rId16"/>
-    <hyperlink ref="Q26" r:id="rId17"/>
-    <hyperlink ref="Q27" r:id="rId18"/>
-    <hyperlink ref="Q28" r:id="rId19"/>
-    <hyperlink ref="Q29" r:id="rId20"/>
-    <hyperlink ref="Q30" r:id="rId21"/>
-    <hyperlink ref="Q31" r:id="rId22"/>
-    <hyperlink ref="Q32" r:id="rId23"/>
-    <hyperlink ref="Q33" r:id="rId24"/>
-    <hyperlink ref="Q34" r:id="rId25"/>
-    <hyperlink ref="Q35" r:id="rId26"/>
-    <hyperlink ref="Q36" r:id="rId27"/>
-    <hyperlink ref="Q37" r:id="rId28"/>
-    <hyperlink ref="Q38" r:id="rId29"/>
-    <hyperlink ref="Q39" r:id="rId30"/>
-    <hyperlink ref="Q40" r:id="rId31"/>
-    <hyperlink ref="Q41" r:id="rId32"/>
-    <hyperlink ref="Q42" r:id="rId33"/>
-    <hyperlink ref="Q12" r:id="rId34"/>
-    <hyperlink ref="Q43" r:id="rId35"/>
-    <hyperlink ref="Q15" r:id="rId36"/>
-    <hyperlink ref="J9" r:id="rId37"/>
-    <hyperlink ref="J8" r:id="rId38"/>
-    <hyperlink ref="J10" r:id="rId39"/>
-    <hyperlink ref="J11" r:id="rId40"/>
-    <hyperlink ref="J13" r:id="rId41"/>
-    <hyperlink ref="J14" r:id="rId42"/>
-    <hyperlink ref="J15" r:id="rId43"/>
-    <hyperlink ref="J16" r:id="rId44"/>
-    <hyperlink ref="J17" r:id="rId45"/>
-    <hyperlink ref="J18" r:id="rId46"/>
-    <hyperlink ref="J19" r:id="rId47"/>
-    <hyperlink ref="J20" r:id="rId48"/>
-    <hyperlink ref="J21" r:id="rId49"/>
-    <hyperlink ref="J22" r:id="rId50"/>
-    <hyperlink ref="J23" r:id="rId51"/>
-    <hyperlink ref="J24" r:id="rId52"/>
-    <hyperlink ref="J25" r:id="rId53"/>
-    <hyperlink ref="J26" r:id="rId54"/>
-    <hyperlink ref="J27" r:id="rId55"/>
-    <hyperlink ref="J28" r:id="rId56"/>
-    <hyperlink ref="J29" r:id="rId57"/>
-    <hyperlink ref="J30" r:id="rId58"/>
-    <hyperlink ref="J31" r:id="rId59"/>
-    <hyperlink ref="J32" r:id="rId60"/>
-    <hyperlink ref="J33" r:id="rId61"/>
-    <hyperlink ref="J34" r:id="rId62"/>
-    <hyperlink ref="J35" r:id="rId63"/>
-    <hyperlink ref="J36" r:id="rId64"/>
-    <hyperlink ref="J37" r:id="rId65"/>
-    <hyperlink ref="J38" r:id="rId66"/>
-    <hyperlink ref="J39" r:id="rId67"/>
-    <hyperlink ref="J40" r:id="rId68"/>
-    <hyperlink ref="J41" r:id="rId69"/>
-    <hyperlink ref="J42" r:id="rId70"/>
-    <hyperlink ref="J43" r:id="rId71"/>
+    <hyperlink ref="J10" r:id="rId1"/>
+    <hyperlink ref="J9" r:id="rId2"/>
+    <hyperlink ref="Q8" r:id="rId3"/>
+    <hyperlink ref="Q9" r:id="rId4"/>
+    <hyperlink ref="Q10" r:id="rId5"/>
+    <hyperlink ref="Q11" r:id="rId6"/>
+    <hyperlink ref="Q12" r:id="rId7"/>
+    <hyperlink ref="Q13" r:id="rId8"/>
+    <hyperlink ref="Q14" r:id="rId9"/>
+    <hyperlink ref="Q15" r:id="rId10"/>
+    <hyperlink ref="Q16" r:id="rId11"/>
+    <hyperlink ref="Q17" r:id="rId12"/>
+    <hyperlink ref="Q18" r:id="rId13"/>
+    <hyperlink ref="Q19" r:id="rId14"/>
+    <hyperlink ref="Q20" r:id="rId15"/>
+    <hyperlink ref="Q21" r:id="rId16"/>
+    <hyperlink ref="Q22" r:id="rId17"/>
+    <hyperlink ref="Q23" r:id="rId18"/>
+    <hyperlink ref="Q24" r:id="rId19"/>
+    <hyperlink ref="Q25" r:id="rId20"/>
+    <hyperlink ref="Q26" r:id="rId21"/>
+    <hyperlink ref="Q27" r:id="rId22"/>
+    <hyperlink ref="Q28" r:id="rId23"/>
+    <hyperlink ref="Q29" r:id="rId24"/>
+    <hyperlink ref="Q30" r:id="rId25"/>
+    <hyperlink ref="Q31" r:id="rId26"/>
+    <hyperlink ref="Q32" r:id="rId27"/>
+    <hyperlink ref="Q33" r:id="rId28"/>
+    <hyperlink ref="Q34" r:id="rId29"/>
+    <hyperlink ref="Q35" r:id="rId30"/>
+    <hyperlink ref="Q36" r:id="rId31"/>
+    <hyperlink ref="Q37" r:id="rId32"/>
+    <hyperlink ref="Q38" r:id="rId33"/>
+    <hyperlink ref="Q39" r:id="rId34"/>
+    <hyperlink ref="Q40" r:id="rId35"/>
+    <hyperlink ref="Q41" r:id="rId36"/>
+    <hyperlink ref="Q42" r:id="rId37"/>
+    <hyperlink ref="Q43" r:id="rId38"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId72"/>
+  <pageSetup orientation="portrait" r:id="rId39"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Cambios que solicita maydeli por whats
</commit_message>
<xml_diff>
--- a/xlsx/a69_f11UPPachuca.xlsx
+++ b/xlsx/a69_f11UPPachuca.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Documents\Dirección de Planeción\2021\SIPOT\RH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Desktop\FRACCIONES COMUNES\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1070,7 +1070,7 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,7 +1084,7 @@
     <col min="7" max="7" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="85.85546875" customWidth="1"/>
+    <col min="10" max="10" width="97.5703125" customWidth="1"/>
     <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="27.5703125" customWidth="1"/>

</xml_diff>

<commit_message>
cambio de nombre y archivos y el 8 a 8a8b
</commit_message>
<xml_diff>
--- a/xlsx/a69_f11UPPachuca.xlsx
+++ b/xlsx/a69_f11UPPachuca.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Documents\Dirección de Planeción\2021\SIPOT\UPP Solventación 1er Trimestre 21\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Documents\Dirección de Planeción\2021\SIPOT\SIPOT 1ER\1er Trimestre 2021 SIPOT  Pagina Oficial UPP\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7065"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8355"/>
   </bookViews>
   <sheets>
     <sheet name="Reporte de Formatos" sheetId="1" r:id="rId1"/>
@@ -754,6 +754,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -764,9 +767,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1051,7 +1051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N2" workbookViewId="0">
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
@@ -1073,7 +1073,7 @@
     <col min="14" max="14" width="41.85546875" customWidth="1"/>
     <col min="15" max="15" width="17.42578125" customWidth="1"/>
     <col min="16" max="16" width="21.5703125" customWidth="1"/>
-    <col min="17" max="17" width="55.7109375" customWidth="1"/>
+    <col min="17" max="17" width="105.28515625" customWidth="1"/>
     <col min="18" max="18" width="73.140625" customWidth="1"/>
     <col min="19" max="19" width="17.5703125" customWidth="1"/>
     <col min="20" max="20" width="20" customWidth="1"/>
@@ -1086,38 +1086,38 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="11" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="11" t="s">
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:21" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="14" t="s">
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1250,29 +1250,29 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
     </row>
     <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1377,10 +1377,10 @@
       <c r="M8" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N8" s="16">
+      <c r="N8" s="11">
         <v>23369.759999999998</v>
       </c>
-      <c r="O8" s="16">
+      <c r="O8" s="11">
         <v>20886.719999999998</v>
       </c>
       <c r="P8" s="2" t="s">
@@ -1440,10 +1440,10 @@
       <c r="M9" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="N9" s="16">
+      <c r="N9" s="11">
         <v>90843.520000000004</v>
       </c>
-      <c r="O9" s="16">
+      <c r="O9" s="11">
         <v>90843.520000000004</v>
       </c>
       <c r="P9" s="2"/>
@@ -1501,10 +1501,10 @@
       <c r="M10" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="N10" s="16">
+      <c r="N10" s="11">
         <v>56102.96</v>
       </c>
-      <c r="O10" s="16">
+      <c r="O10" s="11">
         <v>56102.96</v>
       </c>
       <c r="P10" s="2"/>
@@ -1562,10 +1562,10 @@
       <c r="M11" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="N11" s="16">
+      <c r="N11" s="11">
         <v>39096.32</v>
       </c>
-      <c r="O11" s="16">
+      <c r="O11" s="11">
         <v>34942.400000000001</v>
       </c>
       <c r="P11" s="2" t="s">
@@ -1625,10 +1625,10 @@
       <c r="M12" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N12" s="16">
+      <c r="N12" s="11">
         <v>23369.759999999998</v>
       </c>
-      <c r="O12" s="16">
+      <c r="O12" s="11">
         <v>20886.719999999998</v>
       </c>
       <c r="P12" s="2" t="s">
@@ -1688,10 +1688,10 @@
       <c r="M13" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N13" s="16">
+      <c r="N13" s="11">
         <v>31625.200000000001</v>
       </c>
-      <c r="O13" s="16">
+      <c r="O13" s="11">
         <v>28264.959999999999</v>
       </c>
       <c r="P13" s="2" t="s">
@@ -1751,10 +1751,10 @@
       <c r="M14" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N14" s="16">
+      <c r="N14" s="11">
         <v>31625.200000000001</v>
       </c>
-      <c r="O14" s="16">
+      <c r="O14" s="11">
         <v>28264.959999999999</v>
       </c>
       <c r="P14" s="2" t="s">
@@ -1814,10 +1814,10 @@
       <c r="M15" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N15" s="16">
+      <c r="N15" s="11">
         <v>5415.04</v>
       </c>
-      <c r="O15" s="16">
+      <c r="O15" s="11">
         <v>5415.04</v>
       </c>
       <c r="P15" s="2"/>
@@ -1875,10 +1875,10 @@
       <c r="M16" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N16" s="16">
+      <c r="N16" s="11">
         <v>33276.239999999998</v>
       </c>
-      <c r="O16" s="16">
+      <c r="O16" s="11">
         <v>29740.559999999998</v>
       </c>
       <c r="P16" s="2" t="s">
@@ -1938,10 +1938,10 @@
       <c r="M17" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N17" s="16">
+      <c r="N17" s="11">
         <v>31625.200000000001</v>
       </c>
-      <c r="O17" s="16">
+      <c r="O17" s="11">
         <v>28264.959999999999</v>
       </c>
       <c r="P17" s="2" t="s">
@@ -2001,10 +2001,10 @@
       <c r="M18" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="N18" s="16">
+      <c r="N18" s="11">
         <v>39096.32</v>
       </c>
-      <c r="O18" s="16">
+      <c r="O18" s="11">
         <v>34942.400000000001</v>
       </c>
       <c r="P18" s="2" t="s">
@@ -2064,10 +2064,10 @@
       <c r="M19" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N19" s="16">
+      <c r="N19" s="11">
         <v>31625.200000000001</v>
       </c>
-      <c r="O19" s="16">
+      <c r="O19" s="11">
         <v>28264.959999999999</v>
       </c>
       <c r="P19" s="2" t="s">
@@ -2127,10 +2127,10 @@
       <c r="M20" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="N20" s="16">
+      <c r="N20" s="11">
         <v>37128.720000000001</v>
       </c>
-      <c r="O20" s="16">
+      <c r="O20" s="11">
         <v>33183.68</v>
       </c>
       <c r="P20" s="2" t="s">
@@ -2190,10 +2190,10 @@
       <c r="M21" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N21" s="16">
+      <c r="N21" s="11">
         <v>25020.959999999999</v>
       </c>
-      <c r="O21" s="16">
+      <c r="O21" s="11">
         <v>22362.399999999998</v>
       </c>
       <c r="P21" s="2" t="s">
@@ -2253,10 +2253,10 @@
       <c r="M22" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N22" s="16">
+      <c r="N22" s="11">
         <v>31625.200000000001</v>
       </c>
-      <c r="O22" s="16">
+      <c r="O22" s="11">
         <v>28264.959999999999</v>
       </c>
       <c r="P22" s="2" t="s">
@@ -2316,10 +2316,10 @@
       <c r="M23" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N23" s="16">
+      <c r="N23" s="11">
         <v>28323.040000000001</v>
       </c>
-      <c r="O23" s="16">
+      <c r="O23" s="11">
         <v>25313.68</v>
       </c>
       <c r="P23" s="2" t="s">
@@ -2379,10 +2379,10 @@
       <c r="M24" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N24" s="16">
+      <c r="N24" s="11">
         <v>31625.200000000001</v>
       </c>
-      <c r="O24" s="16">
+      <c r="O24" s="11">
         <v>28264.959999999999</v>
       </c>
       <c r="P24" s="2" t="s">
@@ -2442,10 +2442,10 @@
       <c r="M25" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N25" s="16">
+      <c r="N25" s="11">
         <v>31625.200000000001</v>
       </c>
-      <c r="O25" s="16">
+      <c r="O25" s="11">
         <v>28264.959999999999</v>
       </c>
       <c r="P25" s="2" t="s">
@@ -2505,10 +2505,10 @@
       <c r="M26" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="N26" s="16">
+      <c r="N26" s="11">
         <v>25571.200000000001</v>
       </c>
-      <c r="O26" s="16">
+      <c r="O26" s="11">
         <v>22854.240000000002</v>
       </c>
       <c r="P26" s="2" t="s">
@@ -2568,10 +2568,10 @@
       <c r="M27" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N27" s="16">
+      <c r="N27" s="11">
         <v>33276.239999999998</v>
       </c>
-      <c r="O27" s="16">
+      <c r="O27" s="11">
         <v>29740.559999999998</v>
       </c>
       <c r="P27" s="2" t="s">
@@ -2631,10 +2631,10 @@
       <c r="M28" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="N28" s="16">
+      <c r="N28" s="11">
         <v>37128.720000000001</v>
       </c>
-      <c r="O28" s="16">
+      <c r="O28" s="11">
         <v>33183.68</v>
       </c>
       <c r="P28" s="2" t="s">
@@ -2694,10 +2694,10 @@
       <c r="M29" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N29" s="16">
+      <c r="N29" s="11">
         <v>31625.200000000001</v>
       </c>
-      <c r="O29" s="16">
+      <c r="O29" s="11">
         <v>28264.959999999999</v>
       </c>
       <c r="P29" s="2" t="s">
@@ -2757,10 +2757,10 @@
       <c r="M30" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N30" s="16">
+      <c r="N30" s="11">
         <v>28323.040000000001</v>
       </c>
-      <c r="O30" s="16">
+      <c r="O30" s="11">
         <v>25313.68</v>
       </c>
       <c r="P30" s="2" t="s">
@@ -2820,10 +2820,10 @@
       <c r="M31" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N31" s="16">
+      <c r="N31" s="11">
         <v>31625.200000000001</v>
       </c>
-      <c r="O31" s="16">
+      <c r="O31" s="11">
         <v>28264.959999999999</v>
       </c>
       <c r="P31" s="2" t="s">
@@ -2883,10 +2883,10 @@
       <c r="M32" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N32" s="16">
+      <c r="N32" s="11">
         <v>33276.239999999998</v>
       </c>
-      <c r="O32" s="16">
+      <c r="O32" s="11">
         <v>29740.559999999998</v>
       </c>
       <c r="P32" s="2" t="s">
@@ -2946,10 +2946,10 @@
       <c r="M33" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="N33" s="16">
+      <c r="N33" s="11">
         <v>39096.32</v>
       </c>
-      <c r="O33" s="16">
+      <c r="O33" s="11">
         <v>34942.400000000001</v>
       </c>
       <c r="P33" s="2" t="s">
@@ -3009,10 +3009,10 @@
       <c r="M34" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="N34" s="16">
+      <c r="N34" s="11">
         <v>33276.239999999998</v>
       </c>
-      <c r="O34" s="16">
+      <c r="O34" s="11">
         <v>29740.559999999998</v>
       </c>
       <c r="P34" s="2" t="s">
@@ -3072,10 +3072,10 @@
       <c r="M35" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N35" s="16">
+      <c r="N35" s="11">
         <v>23369.759999999998</v>
       </c>
-      <c r="O35" s="16">
+      <c r="O35" s="11">
         <v>20886.719999999998</v>
       </c>
       <c r="P35" s="2" t="s">
@@ -3135,10 +3135,10 @@
       <c r="M36" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N36" s="16">
+      <c r="N36" s="11">
         <v>31625.200000000001</v>
       </c>
-      <c r="O36" s="16">
+      <c r="O36" s="11">
         <v>28264.959999999999</v>
       </c>
       <c r="P36" s="2" t="s">
@@ -3198,10 +3198,10 @@
       <c r="M37" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N37" s="16">
+      <c r="N37" s="11">
         <v>33276.239999999998</v>
       </c>
-      <c r="O37" s="16">
+      <c r="O37" s="11">
         <v>29740.559999999998</v>
       </c>
       <c r="P37" s="2" t="s">
@@ -3261,10 +3261,10 @@
       <c r="M38" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N38" s="16">
+      <c r="N38" s="11">
         <v>31625.200000000001</v>
       </c>
-      <c r="O38" s="16">
+      <c r="O38" s="11">
         <v>28264.959999999999</v>
       </c>
       <c r="P38" s="2" t="s">
@@ -3324,10 +3324,10 @@
       <c r="M39" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="N39" s="16">
+      <c r="N39" s="11">
         <v>37128.720000000001</v>
       </c>
-      <c r="O39" s="16">
+      <c r="O39" s="11">
         <v>33183.68</v>
       </c>
       <c r="P39" s="2" t="s">
@@ -3387,10 +3387,10 @@
       <c r="M40" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="N40" s="16">
+      <c r="N40" s="11">
         <v>42923.28</v>
       </c>
-      <c r="O40" s="16">
+      <c r="O40" s="11">
         <v>38362.720000000001</v>
       </c>
       <c r="P40" s="2" t="s">
@@ -3450,10 +3450,10 @@
       <c r="M41" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="N41" s="16">
+      <c r="N41" s="11">
         <v>31625.200000000001</v>
       </c>
-      <c r="O41" s="16">
+      <c r="O41" s="11">
         <v>28264.959999999999</v>
       </c>
       <c r="P41" s="2" t="s">
@@ -3513,10 +3513,10 @@
       <c r="M42" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="N42" s="16">
+      <c r="N42" s="11">
         <v>21727.52</v>
       </c>
-      <c r="O42" s="16">
+      <c r="O42" s="11">
         <v>19419.04</v>
       </c>
       <c r="P42" s="2" t="s">
@@ -3576,10 +3576,10 @@
       <c r="M43" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="N43" s="16">
+      <c r="N43" s="11">
         <v>5415.04</v>
       </c>
-      <c r="O43" s="16">
+      <c r="O43" s="11">
         <v>5415.04</v>
       </c>
       <c r="P43" s="2"/>

</xml_diff>